<commit_message>
complex example using a map
</commit_message>
<xml_diff>
--- a/examples-complex/src/test/resources/ComplexBusinessTest.xlsx
+++ b/examples-complex/src/test/resources/ComplexBusinessTest.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="330" windowWidth="21075" windowHeight="9750"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15450" windowHeight="4830"/>
   </bookViews>
   <sheets>
     <sheet name="Test1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="30">
   <si>
     <t>disabled</t>
   </si>
@@ -95,6 +95,15 @@
   </si>
   <si>
     <t>Musterstadt</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>Jane Doe</t>
+  </si>
+  <si>
+    <t>additionalSettings["sex"]</t>
   </si>
 </sst>
 </file>
@@ -458,20 +467,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -479,7 +491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -505,7 +517,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -531,7 +543,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -557,205 +569,361 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
         <v>3</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="4">
+        <v>28288</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>50</v>
+      </c>
+      <c r="H10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="2" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>9</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B21" t="s">
         <v>16</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C21" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D21" s="4">
         <v>26503</v>
       </c>
-      <c r="E18">
+      <c r="E21">
         <v>6</v>
       </c>
-      <c r="F18">
+      <c r="F21">
         <v>100</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G21" t="s">
         <v>19</v>
       </c>
-      <c r="H18">
+      <c r="H21">
         <v>600</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I21" s="7">
         <v>1333.3333</v>
       </c>
-      <c r="J18">
+      <c r="J21">
         <v>1447.3333</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="6"/>
+      <c r="B24" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>22</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B31" t="s">
         <v>17</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C31" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D31" s="4">
         <v>28564</v>
       </c>
-      <c r="E28">
-        <v>2</v>
-      </c>
-      <c r="F28">
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31">
         <v>50</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G31" t="s">
         <v>20</v>
       </c>
-      <c r="H28">
+      <c r="H31">
         <v>100</v>
       </c>
-      <c r="I28">
+      <c r="I31">
         <v>434.7826</v>
       </c>
-      <c r="J28">
+      <c r="J31">
         <v>453.7826</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="4">
+        <v>28288</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40">
+        <v>50</v>
+      </c>
+      <c r="G40" t="s">
+        <v>20</v>
+      </c>
+      <c r="H40">
+        <v>100</v>
+      </c>
+      <c r="I40">
+        <v>434.7826</v>
+      </c>
+      <c r="J40">
+        <v>444.70694800000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new feature: use expression for accessing an element out of a collection instead of the index.
</commit_message>
<xml_diff>
--- a/examples-complex/src/test/resources/ComplexBusinessTest.xlsx
+++ b/examples-complex/src/test/resources/ComplexBusinessTest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="31">
   <si>
     <t>disabled</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>additionalSettings["sex"]</t>
+  </si>
+  <si>
+    <t>list[name=John].count</t>
   </si>
 </sst>
 </file>
@@ -467,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,7 +834,7 @@
         <v>453.7826</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
@@ -841,7 +844,7 @@
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -849,7 +852,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>2</v>
       </c>
@@ -857,12 +860,12 @@
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>2</v>
       </c>
@@ -893,8 +896,11 @@
       <c r="J39" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K39" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -924,6 +930,9 @@
       </c>
       <c r="J40">
         <v>444.70694800000001</v>
+      </c>
+      <c r="K40">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>